<commit_message>
&&& №10265 от 25.03.2024 https://2eurostore.ru/
</commit_message>
<xml_diff>
--- a/Collections/EURO/Austria/#EURO#Austria#Commemorative#[2005-present]#UNC%varieties.xlsx
+++ b/Collections/EURO/Austria/#EURO#Austria#Commemorative#[2005-present]#UNC%varieties.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Lord_Alexator\Documents\CoinCollection\Collections\EURO\Austria\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A3B2AE45-0798-46EA-81AC-4821DEAAA6E0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3C28360F-B95A-4231-B9BE-4548A0673ED4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5730" yWindow="780" windowWidth="28800" windowHeight="17750" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="38620" windowHeight="21220" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="2€" sheetId="1" r:id="rId1"/>
@@ -789,7 +789,7 @@
       <pane xSplit="7" ySplit="2" topLeftCell="H3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="F1" sqref="F1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="B1" sqref="B1:B2"/>
+      <selection pane="bottomRight" activeCell="H23" sqref="H23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.35"/>
@@ -1268,7 +1268,7 @@
         <v>2590000</v>
       </c>
       <c r="F20" s="10">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G20" s="11" t="str">
         <f t="shared" si="1"/>

</xml_diff>